<commit_message>
se hacen cambios y se agrega generador de llaves a admin
</commit_message>
<xml_diff>
--- a/data/excel/horarios/exprebus-38-sabados-sn.xlsx
+++ b/data/excel/horarios/exprebus-38-sabados-sn.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRACTICAS WEB\NEXT\horabondi\data\excel\horarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PRACTICAS WEB\NEXT\horabondi\docs\exprebus\horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97D96F67-0EED-434C-9D93-7EA7F25A2085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C6E4D3-B570-4D6C-BB58-D5741FE7C25F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="3165" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="22-09-2022" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>

</xml_diff>